<commit_message>
Fix problems with update from Menu.x, now its works
</commit_message>
<xml_diff>
--- a/application/admin/Menu.xlsx
+++ b/application/admin/Menu.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
   <si>
     <r>
       <rPr>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Рамен на нежном сливочном рыбном бульоне, с добавлением маринованного угря, грибов муэр, кунжута, зеленого лука</t>
+  </si>
+  <si>
+    <t>45642981-18cb-4716-9cce-4ec65f149555</t>
   </si>
   <si>
     <t>Чиизу Рамен</t>
@@ -1354,7 +1357,7 @@
   <cols>
     <col min="1" max="1" width="7.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.125" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="77.6719" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
@@ -1487,13 +1490,13 @@
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" t="s" s="6">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s" s="7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F9" s="9">
         <v>132.88</v>
@@ -1504,10 +1507,10 @@
         <v>21</v>
       </c>
       <c r="B10" t="s" s="3">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s" s="3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="11"/>
@@ -1516,13 +1519,13 @@
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="5"/>
       <c r="B11" t="s" s="6">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s" s="3">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s" s="7">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="11"/>
       <c r="F11" s="5"/>
@@ -1531,13 +1534,13 @@
       <c r="A12" s="5"/>
       <c r="B12" s="12"/>
       <c r="C12" t="s" s="13">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="7">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s" s="8">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F12" s="9">
         <v>2700.79</v>
@@ -1547,13 +1550,13 @@
       <c r="A13" s="5"/>
       <c r="B13" s="12"/>
       <c r="C13" t="s" s="13">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s" s="7">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F13" s="9">
         <v>3100.33</v>
@@ -1563,13 +1566,13 @@
       <c r="A14" s="5"/>
       <c r="B14" s="12"/>
       <c r="C14" t="s" s="13">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s" s="7">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E14" t="s" s="8">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F14" s="9">
         <v>1850.42</v>
@@ -1578,13 +1581,13 @@
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="5"/>
       <c r="B15" t="s" s="6">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s" s="3">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15" t="s" s="7">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="5"/>
@@ -1593,13 +1596,13 @@
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" t="s" s="6">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16" t="s" s="7">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s" s="8">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F16" s="9">
         <v>420.78</v>
@@ -1609,13 +1612,13 @@
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" t="s" s="6">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E17" t="s" s="8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F17" s="9">
         <v>440.11</v>
@@ -1625,13 +1628,13 @@
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" t="s" s="6">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s" s="7">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s" s="8">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F18" s="9">
         <v>520.08</v>

</xml_diff>

<commit_message>
Add show price with discount
</commit_message>
<xml_diff>
--- a/application/admin/Menu.xlsx
+++ b/application/admin/Menu.xlsx
@@ -186,7 +186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -212,6 +212,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <i val="1"/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Montserrat"/>
     </font>
   </fonts>
   <fills count="3">
@@ -257,7 +264,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -290,6 +297,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -1349,7 +1359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1357,11 +1367,11 @@
   <cols>
     <col min="1" max="1" width="7.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.8516" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.1719" style="1" customWidth="1"/>
     <col min="4" max="4" width="21.6719" style="1" customWidth="1"/>
     <col min="5" max="5" width="77.6719" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="12.5" style="1" customWidth="1"/>
+    <col min="6" max="7" width="12.5" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1377,6 +1387,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="5"/>
@@ -1391,6 +1402,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="5"/>
@@ -1407,6 +1419,9 @@
       <c r="F3" s="9">
         <v>182.99</v>
       </c>
+      <c r="G3" s="9">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
       <c r="A4" s="5"/>
@@ -1423,6 +1438,9 @@
       <c r="F4" s="9">
         <v>215.36</v>
       </c>
+      <c r="G4" s="11">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="5"/>
@@ -1439,6 +1457,9 @@
       <c r="F5" s="9">
         <v>265.57</v>
       </c>
+      <c r="G5" s="9">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5"/>
@@ -1451,8 +1472,9 @@
       <c r="D6" t="s" s="7">
         <v>17</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="12"/>
       <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="5"/>
@@ -1469,6 +1491,9 @@
       <c r="F7" s="9">
         <v>166.47</v>
       </c>
+      <c r="G7" s="9">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="5"/>
@@ -1485,6 +1510,9 @@
       <c r="F8" s="9">
         <v>168.25</v>
       </c>
+      <c r="G8" s="9">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="5"/>
@@ -1501,6 +1529,9 @@
       <c r="F9" s="9">
         <v>132.88</v>
       </c>
+      <c r="G9" s="9">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" t="s" s="6">
@@ -1513,8 +1544,9 @@
         <v>28</v>
       </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="11"/>
+      <c r="E10" s="12"/>
       <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="5"/>
@@ -1527,13 +1559,14 @@
       <c r="D11" t="s" s="7">
         <v>31</v>
       </c>
-      <c r="E11" s="11"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="5"/>
-      <c r="B12" s="12"/>
-      <c r="C12" t="s" s="13">
+      <c r="B12" s="13"/>
+      <c r="C12" t="s" s="14">
         <v>32</v>
       </c>
       <c r="D12" t="s" s="7">
@@ -1544,12 +1577,15 @@
       </c>
       <c r="F12" s="9">
         <v>2700.79</v>
+      </c>
+      <c r="G12" s="9">
+        <v>90</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="5"/>
-      <c r="B13" s="12"/>
-      <c r="C13" t="s" s="13">
+      <c r="B13" s="13"/>
+      <c r="C13" t="s" s="14">
         <v>35</v>
       </c>
       <c r="D13" t="s" s="7">
@@ -1560,12 +1596,15 @@
       </c>
       <c r="F13" s="9">
         <v>3100.33</v>
+      </c>
+      <c r="G13" s="9">
+        <v>90</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="5"/>
-      <c r="B14" s="12"/>
-      <c r="C14" t="s" s="13">
+      <c r="B14" s="13"/>
+      <c r="C14" t="s" s="14">
         <v>38</v>
       </c>
       <c r="D14" t="s" s="7">
@@ -1576,6 +1615,9 @@
       </c>
       <c r="F14" s="9">
         <v>1850.42</v>
+      </c>
+      <c r="G14" s="9">
+        <v>90</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
@@ -1589,8 +1631,9 @@
       <c r="D15" t="s" s="7">
         <v>43</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="5"/>
@@ -1607,6 +1650,9 @@
       <c r="F16" s="9">
         <v>420.78</v>
       </c>
+      <c r="G16" s="9">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="5"/>
@@ -1623,6 +1669,9 @@
       <c r="F17" s="9">
         <v>440.11</v>
       </c>
+      <c r="G17" s="9">
+        <v>90</v>
+      </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="5"/>
@@ -1639,6 +1688,7 @@
       <c r="F18" s="9">
         <v>520.08</v>
       </c>
+      <c r="G18" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>